<commit_message>
DWH-11: Complete type conversion in import batch job
</commit_message>
<xml_diff>
--- a/common/src/test/resources/spends.xlsx
+++ b/common/src/test/resources/spends.xlsx
@@ -699,15 +699,15 @@
   <dimension ref="A1:AO427"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A338" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AN99" activeCellId="0" sqref="AN99"/>
+      <selection pane="topLeft" activeCell="M360" activeCellId="0" sqref="M360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="28.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25.17"/>

</xml_diff>